<commit_message>
Agregados todos los tests al paper
</commit_message>
<xml_diff>
--- a/Implementación/Test 10/decisiones_w2.xlsx
+++ b/Implementación/Test 10/decisiones_w2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCLAMR\OneDrive\OneDrive - MIC\Documents\GitHub\Tesis\Implementación\Test 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1020B64-41D9-42CC-92A0-84CBB0F3CB4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBEEFA70-942C-4424-A132-49CC97A4BEC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2175" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{33A03FC3-5BAD-44A0-94E7-F0B586E9549A}"/>
   </bookViews>
@@ -83,6 +83,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,14 +434,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EA9497-E300-4BA0-8FA4-AAF0951F4AA0}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -470,13 +478,13 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>6.3262869855948978E-3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>7.9523737534916616</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0.82878220639442401</v>
       </c>
     </row>
@@ -490,13 +498,13 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>3.6605416353111819E-3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>7.9173378416528148</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.86968941803362243</v>
       </c>
     </row>
@@ -510,13 +518,13 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>3.6605416353111819E-3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>7.9173378416528148</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.86968941803362243</v>
       </c>
     </row>
@@ -530,13 +538,13 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1.028933219780348E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>7.9751970031290176</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>0.78624356849034693</v>
       </c>
     </row>
@@ -550,13 +558,13 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>6.3262869855948978E-3</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>7.9523737534916616</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0.82878220639442401</v>
       </c>
     </row>
@@ -570,13 +578,13 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1.028933219780348E-2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>7.9751970031290176</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0.78624356849034693</v>
       </c>
     </row>
@@ -590,13 +598,13 @@
       <c r="C8">
         <v>661</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>7.4913065631597417</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>0.99933023386704944</v>
       </c>
     </row>
@@ -610,13 +618,13 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>0.83101514558681666</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>7.9895651313096439</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>0.75065436358303694</v>
       </c>
     </row>

</xml_diff>